<commit_message>
fine tune with OnlineContrastiveLoss implementation
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\workspaces\nlp\wc-sbert\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56ECFCB5-E142-4642-BDF9-E276B9C481D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2FF18E-5F33-4F8C-937D-716FC5B71575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="4665" windowWidth="29040" windowHeight="16440" xr2:uid="{5DD896CD-0F37-47FF-B777-3EFC268D410F}"/>
+    <workbookView xWindow="-25710" yWindow="-2140" windowWidth="25820" windowHeight="16220" xr2:uid="{5DD896CD-0F37-47FF-B777-3EFC268D410F}"/>
   </bookViews>
   <sheets>
     <sheet name="AGNEWS" sheetId="6" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="dbpedia" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="46">
   <si>
     <t>i0</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -168,13 +169,49 @@
     <t>測試 threshold</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>loss function</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mnr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. threshold 0.9 完全不會增加 samples</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. online contrast loss 看起來才是對的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. descritive label 只適用於 finetune, 不適合拿來做 inference</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>測試 online contrastive loss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>online contrastive loss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>測試 batch size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="180" formatCode="#,##0_ "/>
+    <numFmt numFmtId="176" formatCode="#,##0_ "/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -200,7 +237,7 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,6 +259,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -292,7 +335,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -308,16 +351,40 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -329,12 +396,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -343,9 +404,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -365,7 +423,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -420,7 +478,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-TW"/>
-              <a:t>AGNEWS-11130945</a:t>
+              <a:t>AGNEWS-11141717</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -465,7 +523,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>AGNEWS!$C$7</c:f>
+              <c:f>AGNEWS!$C$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -488,7 +546,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>AGNEWS!$C$8:$C$17</c:f>
+              <c:f>AGNEWS!$C$9:$C$18</c:f>
               <c:numCache>
                 <c:formatCode>#,##0_ </c:formatCode>
                 <c:ptCount val="10"/>
@@ -496,31 +554,31 @@
                   <c:v>1877</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>697</c:v>
+                  <c:v>619</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>513</c:v>
+                  <c:v>839</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>521</c:v>
+                  <c:v>533</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>702</c:v>
+                  <c:v>1715</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1388</c:v>
+                  <c:v>2472</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2506</c:v>
+                  <c:v>5034</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6594</c:v>
+                  <c:v>28156</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>22964</c:v>
+                  <c:v>125600</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>152434</c:v>
+                  <c:v>725003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -553,7 +611,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>AGNEWS!$D$7</c:f>
+              <c:f>AGNEWS!$D$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -576,39 +634,39 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>AGNEWS!$D$8:$D$17</c:f>
+              <c:f>AGNEWS!$D$9:$D$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.77669999999999995</c:v>
+                  <c:v>0.77629999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.77969999999999995</c:v>
+                  <c:v>0.78200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.78339999999999999</c:v>
+                  <c:v>0.78620000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.78669999999999995</c:v>
+                  <c:v>0.79449999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.7913</c:v>
+                  <c:v>0.80030000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.80100000000000005</c:v>
+                  <c:v>0.80969999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.80769999999999997</c:v>
+                  <c:v>0.80379999999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.8085</c:v>
+                  <c:v>0.79700000000000004</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.80030000000000001</c:v>
+                  <c:v>0.80079999999999996</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.79800000000000004</c:v>
+                  <c:v>0.78949999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -792,6 +850,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="360945872"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -971,7 +1030,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>AGNEWS!$I$7</c:f>
+              <c:f>AGNEWS!$I$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -994,7 +1053,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>AGNEWS!$I$8:$I$17</c:f>
+              <c:f>AGNEWS!$I$9:$I$18</c:f>
               <c:numCache>
                 <c:formatCode>#,##0_ </c:formatCode>
                 <c:ptCount val="10"/>
@@ -1059,7 +1118,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>AGNEWS!$J$7</c:f>
+              <c:f>AGNEWS!$J$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1082,7 +1141,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>AGNEWS!$J$8:$J$17</c:f>
+              <c:f>AGNEWS!$J$9:$J$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1131,7 +1190,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>AGNEWS!$K$7</c:f>
+              <c:f>AGNEWS!$K$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1154,7 +1213,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>AGNEWS!$K$8:$K$17</c:f>
+              <c:f>AGNEWS!$K$9:$K$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1539,7 +1598,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>AGNEWS!$F$7</c:f>
+              <c:f>AGNEWS!$F$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1562,7 +1621,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>AGNEWS!$F$8:$F$17</c:f>
+              <c:f>AGNEWS!$F$9:$F$18</c:f>
               <c:numCache>
                 <c:formatCode>#,##0_ </c:formatCode>
                 <c:ptCount val="10"/>
@@ -1627,7 +1686,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>AGNEWS!$G$7</c:f>
+              <c:f>AGNEWS!$G$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1650,7 +1709,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>AGNEWS!$G$8:$G$17</c:f>
+              <c:f>AGNEWS!$G$9:$G$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1980,6 +2039,513 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-TW"/>
+              <a:t>AGNEWS-11142154</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>AGNEWS!$Q$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>新增筆數</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>AGNEWS!$Q$9:$Q$18</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0_ </c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9385</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11140</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21425</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51075</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>118360</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>894110</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2455315</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2226005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1327315</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2AFC-4BF6-B809-8619CF4C5107}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="120682624"/>
+        <c:axId val="120683872"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>AGNEWS!$R$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>準確率</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>AGNEWS!$R$9:$R$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.82579999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.82789999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.82620000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.83489999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.82010000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.80640000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.78280000000000005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.75890000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.75629999999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.73050000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2AFC-4BF6-B809-8619CF4C5107}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="361640208"/>
+        <c:axId val="360945872"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="120682624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="120683872"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="120683872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0_ " sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="120682624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="360945872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="361640208"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="361640208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="360945872"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst>
+      <a:glow rad="12700">
+        <a:schemeClr val="accent1">
+          <a:alpha val="40000"/>
+        </a:schemeClr>
+      </a:glow>
+      <a:outerShdw blurRad="50800" dist="50800" dir="600000" algn="ctr" rotWithShape="0">
+        <a:srgbClr val="000000">
+          <a:alpha val="43137"/>
+        </a:srgbClr>
+      </a:outerShdw>
+    </a:effectLst>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-TW"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -2400,7 +2966,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-TW"/>
@@ -2848,6 +3414,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="2081050016"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2905,7 +3472,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-TW"/>
@@ -3339,7 +3906,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-TW"/>
@@ -4053,6 +4620,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -5563,7 +6170,7 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -7072,6 +7679,509 @@
 </file>
 
 <file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7580,13 +8690,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>333374</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>4760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>475799</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>160610</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7618,13 +8728,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>466275</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>146325</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7656,13 +8766,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>190050</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>155850</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7685,6 +8795,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>3175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>91625</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>162200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="圖表 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BC05CF0-6106-4D11-A8B4-87762C9E5A74}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8156,10 +9304,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F93FB416-C36E-4E64-BE2B-23308EA3B2C9}">
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:U38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -8178,791 +9326,1144 @@
     <col min="12" max="12" width="11.25" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.75" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="9">
-        <v>11130945</v>
-      </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="9">
+      <c r="B1" s="17">
+        <v>11141717</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="17">
         <v>11141112</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="4">
+      <c r="F1" s="18"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="15">
         <v>11131802</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4">
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15">
         <v>11141317</v>
       </c>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15">
+        <v>11142154</v>
+      </c>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15">
+        <v>11152050</v>
+      </c>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
     </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:21" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="14" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="6" t="s">
+      <c r="F2" s="21"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6" t="s">
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="T2" s="24"/>
+      <c r="U2" s="25"/>
     </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="21">
-        <v>0.85</v>
-      </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="24">
-        <v>0.85</v>
+    <row r="3" spans="1:21" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="21"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="23" t="s">
+        <v>38</v>
       </c>
       <c r="M3" s="24"/>
       <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="T3" s="24"/>
+      <c r="U3" s="25"/>
     </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:21" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="26">
+        <v>0.85</v>
+      </c>
+      <c r="F4" s="27"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="16">
+        <v>0.85</v>
+      </c>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="23">
+        <v>0.8</v>
+      </c>
+      <c r="T4" s="24"/>
+      <c r="U4" s="25"/>
+    </row>
+    <row r="5" spans="1:21" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B5" s="14">
         <v>128</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="18">
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="23">
         <v>128</v>
       </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="6">
+      <c r="F5" s="24"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="14">
         <v>128</v>
       </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6">
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14">
         <v>128</v>
       </c>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14">
+        <v>128</v>
+      </c>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="16">
+        <v>256</v>
+      </c>
+      <c r="T5" s="16"/>
+      <c r="U5" s="16"/>
     </row>
-    <row r="5" spans="1:15" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="6" spans="1:21" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B6" s="14">
         <v>128</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="18">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="23">
         <v>128</v>
       </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="6">
+      <c r="F6" s="24"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="14">
         <v>128</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6">
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14">
         <v>128</v>
       </c>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14">
+        <v>128</v>
+      </c>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="23">
+        <v>128</v>
+      </c>
+      <c r="T6" s="24"/>
+      <c r="U6" s="25"/>
     </row>
-    <row r="6" spans="1:15" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="7" spans="1:21" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B7" s="14">
         <v>1</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="18">
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="23">
         <v>1</v>
       </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="6">
+      <c r="F7" s="24"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="14">
         <v>1</v>
       </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6">
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14">
         <v>1</v>
       </c>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="23">
+        <v>1</v>
+      </c>
+      <c r="T7" s="24"/>
+      <c r="U7" s="25"/>
     </row>
-    <row r="7" spans="1:15" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="8" spans="1:21" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="J8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="K7" s="13" t="s">
+      <c r="K8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="L8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="M8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="N7" s="13" t="s">
+      <c r="N8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="O7" s="13" t="s">
+      <c r="O8" s="8" t="s">
         <v>35</v>
       </c>
+      <c r="P8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="R8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="S8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="T8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="U8" s="8" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="8" spans="1:15" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="9" spans="1:21" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B9" s="7">
         <v>1877</v>
       </c>
-      <c r="C8" s="12">
-        <f>B8</f>
+      <c r="C9" s="7">
+        <f>B9</f>
         <v>1877</v>
       </c>
-      <c r="D8" s="7">
-        <v>0.77669999999999995</v>
-      </c>
-      <c r="E8" s="12">
+      <c r="D9" s="5">
+        <v>0.77629999999999999</v>
+      </c>
+      <c r="E9" s="7">
         <v>241</v>
       </c>
-      <c r="F8" s="12">
-        <f>E8</f>
+      <c r="F9" s="7">
+        <f>E9</f>
         <v>241</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G9" s="5">
         <v>0.78359999999999996</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H9" s="7">
         <v>333</v>
       </c>
-      <c r="I8" s="12">
-        <f>H8</f>
+      <c r="I9" s="7">
+        <f>H9</f>
         <v>333</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J9" s="5">
         <v>0.7863</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K9" s="5">
         <v>0.75749999999999995</v>
       </c>
-      <c r="L8" s="12">
+      <c r="L9" s="7">
         <v>27</v>
       </c>
-      <c r="M8" s="12">
-        <f>L8</f>
+      <c r="M9" s="7">
+        <f>L9</f>
         <v>27</v>
       </c>
-      <c r="N8" s="7">
+      <c r="N9" s="5">
         <v>0.77239999999999998</v>
       </c>
-      <c r="O8" s="7">
+      <c r="O9" s="5">
         <v>0.74639999999999995</v>
       </c>
+      <c r="P9" s="7">
+        <v>9385</v>
+      </c>
+      <c r="Q9" s="7">
+        <f>P9</f>
+        <v>9385</v>
+      </c>
+      <c r="R9" s="5">
+        <v>0.82579999999999998</v>
+      </c>
+      <c r="S9" s="10">
+        <v>9385</v>
+      </c>
+      <c r="T9" s="10">
+        <f>S9</f>
+        <v>9385</v>
+      </c>
+      <c r="U9" s="10">
+        <v>0.83130000000000004</v>
+      </c>
     </row>
-    <row r="9" spans="1:15" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="10" spans="1:21" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="12">
-        <v>2574</v>
-      </c>
-      <c r="C9" s="12">
-        <f t="shared" ref="C9:C17" si="0">B9-B8</f>
-        <v>697</v>
-      </c>
-      <c r="D9" s="7">
-        <v>0.77969999999999995</v>
-      </c>
-      <c r="E9" s="12">
+      <c r="B10" s="7">
+        <v>2496</v>
+      </c>
+      <c r="C10" s="7">
+        <f t="shared" ref="C10:C18" si="0">B10-B9</f>
+        <v>619</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="E10" s="7">
         <v>633</v>
       </c>
-      <c r="F9" s="12">
-        <f>E9-E8</f>
+      <c r="F10" s="7">
+        <f>E10-E9</f>
         <v>392</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G10" s="5">
         <v>0.80679999999999996</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H10" s="7">
         <v>805</v>
       </c>
-      <c r="I9" s="12">
-        <f>H9-H8</f>
+      <c r="I10" s="7">
+        <f>H10-H9</f>
         <v>472</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J10" s="5">
         <v>0.79759999999999998</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K10" s="5">
         <v>0.78029999999999999</v>
       </c>
-      <c r="L9" s="12">
+      <c r="L10" s="7">
         <v>27</v>
       </c>
-      <c r="M9" s="12">
-        <f>L9-L8</f>
+      <c r="M10" s="7">
+        <f>L10-L9</f>
         <v>0</v>
       </c>
-      <c r="N9" s="7">
+      <c r="N10" s="5">
         <v>0.77239999999999998</v>
       </c>
-      <c r="O9" s="7">
+      <c r="O10" s="5">
         <v>0.74639999999999995</v>
       </c>
+      <c r="P10" s="7">
+        <v>20525</v>
+      </c>
+      <c r="Q10" s="7">
+        <f>P10-P9</f>
+        <v>11140</v>
+      </c>
+      <c r="R10" s="5">
+        <v>0.82789999999999997</v>
+      </c>
+      <c r="S10" s="10">
+        <v>24215</v>
+      </c>
+      <c r="T10" s="10">
+        <f>S10-S9</f>
+        <v>14830</v>
+      </c>
+      <c r="U10" s="10">
+        <v>0.83299999999999996</v>
+      </c>
     </row>
-    <row r="10" spans="1:15" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="11" spans="1:21" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="12">
-        <v>3087</v>
-      </c>
-      <c r="C10" s="12">
+      <c r="B11" s="7">
+        <v>3335</v>
+      </c>
+      <c r="C11" s="7">
         <f t="shared" si="0"/>
-        <v>513</v>
-      </c>
-      <c r="D10" s="7">
-        <v>0.78339999999999999</v>
-      </c>
-      <c r="E10" s="12">
+        <v>839</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0.78620000000000001</v>
+      </c>
+      <c r="E11" s="7">
         <v>2653</v>
       </c>
-      <c r="F10" s="12">
-        <f t="shared" ref="F10:F17" si="1">E10-E9</f>
+      <c r="F11" s="7">
+        <f t="shared" ref="F11:F18" si="1">E11-E10</f>
         <v>2020</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G11" s="5">
         <v>0.80930000000000002</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H11" s="7">
         <v>3941</v>
       </c>
-      <c r="I10" s="12">
-        <f t="shared" ref="I10:I17" si="2">H10-H9</f>
+      <c r="I11" s="7">
+        <f t="shared" ref="I11:I18" si="2">H11-H10</f>
         <v>3136</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J11" s="5">
         <v>0.80930000000000002</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K11" s="5">
         <v>0.78659999999999997</v>
       </c>
-      <c r="L10" s="12">
+      <c r="L11" s="7">
         <v>27</v>
       </c>
-      <c r="M10" s="12">
-        <f t="shared" ref="M10:M17" si="3">L10-L9</f>
+      <c r="M11" s="7">
+        <f t="shared" ref="M11:M18" si="3">L11-L10</f>
         <v>0</v>
       </c>
-      <c r="N10" s="7">
+      <c r="N11" s="5">
         <v>0.77239999999999998</v>
       </c>
-      <c r="O10" s="7">
+      <c r="O11" s="5">
         <v>0.74639999999999995</v>
       </c>
+      <c r="P11" s="7">
+        <v>41950</v>
+      </c>
+      <c r="Q11" s="7">
+        <f t="shared" ref="Q11:Q18" si="4">P11-P10</f>
+        <v>21425</v>
+      </c>
+      <c r="R11" s="5">
+        <v>0.82620000000000005</v>
+      </c>
+      <c r="S11" s="10">
+        <v>29765</v>
+      </c>
+      <c r="T11" s="10">
+        <f t="shared" ref="T11:T18" si="5">S11-S10</f>
+        <v>5550</v>
+      </c>
+      <c r="U11" s="29">
+        <v>0.84079999999999999</v>
+      </c>
     </row>
-    <row r="11" spans="1:15" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="12" spans="1:21" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="12">
-        <v>3608</v>
-      </c>
-      <c r="C11" s="12">
+      <c r="B12" s="7">
+        <v>3868</v>
+      </c>
+      <c r="C12" s="7">
         <f t="shared" si="0"/>
-        <v>521</v>
-      </c>
-      <c r="D11" s="7">
-        <v>0.78669999999999995</v>
-      </c>
-      <c r="E11" s="12">
+        <v>533</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0.79449999999999998</v>
+      </c>
+      <c r="E12" s="7">
         <v>3095</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F12" s="7">
         <f t="shared" si="1"/>
         <v>442</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G12" s="5">
         <v>0.81079999999999997</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H12" s="7">
         <v>5376</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I12" s="7">
         <f t="shared" si="2"/>
         <v>1435</v>
       </c>
-      <c r="J11" s="17">
+      <c r="J12" s="9">
         <v>0.82079999999999997</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K12" s="5">
         <v>0.79010000000000002</v>
       </c>
-      <c r="L11" s="12">
+      <c r="L12" s="7">
         <v>27</v>
       </c>
-      <c r="M11" s="12">
+      <c r="M12" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N11" s="7">
+      <c r="N12" s="5">
         <v>0.77239999999999998</v>
       </c>
-      <c r="O11" s="7">
+      <c r="O12" s="5">
         <v>0.74639999999999995</v>
       </c>
+      <c r="P12" s="7">
+        <v>93025</v>
+      </c>
+      <c r="Q12" s="7">
+        <f t="shared" si="4"/>
+        <v>51075</v>
+      </c>
+      <c r="R12" s="12">
+        <v>0.83489999999999998</v>
+      </c>
+      <c r="S12" s="10">
+        <v>37590</v>
+      </c>
+      <c r="T12" s="10">
+        <f t="shared" si="5"/>
+        <v>7825</v>
+      </c>
+      <c r="U12" s="10">
+        <v>0.83330000000000004</v>
+      </c>
     </row>
-    <row r="12" spans="1:15" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    <row r="13" spans="1:21" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="12">
-        <v>4310</v>
-      </c>
-      <c r="C12" s="12">
+      <c r="B13" s="7">
+        <v>5583</v>
+      </c>
+      <c r="C13" s="7">
         <f t="shared" si="0"/>
-        <v>702</v>
-      </c>
-      <c r="D12" s="7">
-        <v>0.7913</v>
-      </c>
-      <c r="E12" s="12">
+        <v>1715</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0.80030000000000001</v>
+      </c>
+      <c r="E13" s="7">
         <v>3518</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F13" s="7">
         <f t="shared" si="1"/>
         <v>423</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G13" s="5">
         <v>0.8125</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H13" s="7">
         <v>9258</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I13" s="7">
         <f t="shared" si="2"/>
         <v>3882</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J13" s="5">
         <v>0.81830000000000003</v>
       </c>
-      <c r="K12" s="17">
+      <c r="K13" s="9">
         <v>0.79430000000000001</v>
       </c>
-      <c r="L12" s="12">
+      <c r="L13" s="7">
         <v>27</v>
       </c>
-      <c r="M12" s="12">
+      <c r="M13" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N12" s="7">
+      <c r="N13" s="5">
         <v>0.77239999999999998</v>
       </c>
-      <c r="O12" s="7">
+      <c r="O13" s="5">
         <v>0.74639999999999995</v>
       </c>
+      <c r="P13" s="7">
+        <v>163525</v>
+      </c>
+      <c r="Q13" s="7">
+        <f t="shared" si="4"/>
+        <v>70500</v>
+      </c>
+      <c r="R13" s="5">
+        <v>0.82010000000000005</v>
+      </c>
+      <c r="S13" s="10">
+        <v>50350</v>
+      </c>
+      <c r="T13" s="10">
+        <f t="shared" si="5"/>
+        <v>12760</v>
+      </c>
+      <c r="U13" s="10">
+        <v>0.83109999999999995</v>
+      </c>
     </row>
-    <row r="13" spans="1:15" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+    <row r="14" spans="1:21" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="12">
-        <v>5698</v>
-      </c>
-      <c r="C13" s="12">
+      <c r="B14" s="7">
+        <v>8055</v>
+      </c>
+      <c r="C14" s="7">
         <f t="shared" si="0"/>
-        <v>1388</v>
-      </c>
-      <c r="D13" s="7">
-        <v>0.80100000000000005</v>
-      </c>
-      <c r="E13" s="12">
+        <v>2472</v>
+      </c>
+      <c r="D14" s="12">
+        <v>0.80969999999999998</v>
+      </c>
+      <c r="E14" s="7">
         <v>4024</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F14" s="7">
         <f t="shared" si="1"/>
         <v>506</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G14" s="5">
         <v>0.81340000000000001</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H14" s="7">
         <v>18459</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I14" s="7">
         <f t="shared" si="2"/>
         <v>9201</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J14" s="5">
         <v>0.79749999999999999</v>
       </c>
-      <c r="K13" s="7">
+      <c r="K14" s="5">
         <v>0.77859999999999996</v>
       </c>
-      <c r="L13" s="12">
+      <c r="L14" s="7">
         <v>27</v>
       </c>
-      <c r="M13" s="12">
+      <c r="M14" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N13" s="7">
+      <c r="N14" s="5">
         <v>0.77239999999999998</v>
       </c>
-      <c r="O13" s="7">
+      <c r="O14" s="5">
         <v>0.74639999999999995</v>
       </c>
+      <c r="P14" s="7">
+        <v>281885</v>
+      </c>
+      <c r="Q14" s="7">
+        <f t="shared" si="4"/>
+        <v>118360</v>
+      </c>
+      <c r="R14" s="5">
+        <v>0.80640000000000001</v>
+      </c>
+      <c r="S14" s="10">
+        <v>66105</v>
+      </c>
+      <c r="T14" s="10">
+        <f t="shared" si="5"/>
+        <v>15755</v>
+      </c>
+      <c r="U14" s="10">
+        <v>0.82640000000000002</v>
+      </c>
     </row>
-    <row r="14" spans="1:15" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+    <row r="15" spans="1:21" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="12">
-        <v>8204</v>
-      </c>
-      <c r="C14" s="12">
+      <c r="B15" s="7">
+        <v>13089</v>
+      </c>
+      <c r="C15" s="7">
         <f t="shared" si="0"/>
-        <v>2506</v>
-      </c>
-      <c r="D14" s="7">
-        <v>0.80769999999999997</v>
-      </c>
-      <c r="E14" s="12">
+        <v>5034</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0.80379999999999996</v>
+      </c>
+      <c r="E15" s="7">
         <v>4888</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F15" s="7">
         <f t="shared" si="1"/>
         <v>864</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G15" s="5">
         <v>0.81659999999999999</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H15" s="7">
         <v>62119</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I15" s="7">
         <f t="shared" si="2"/>
         <v>43660</v>
       </c>
-      <c r="J14" s="7">
+      <c r="J15" s="5">
         <v>0.77529999999999999</v>
       </c>
-      <c r="K14" s="7">
+      <c r="K15" s="5">
         <v>0.76790000000000003</v>
       </c>
-      <c r="L14" s="12">
+      <c r="L15" s="7">
         <v>27</v>
       </c>
-      <c r="M14" s="12">
+      <c r="M15" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N14" s="7">
+      <c r="N15" s="5">
         <v>0.77239999999999998</v>
       </c>
-      <c r="O14" s="7">
+      <c r="O15" s="5">
         <v>0.74639999999999995</v>
       </c>
+      <c r="P15" s="7">
+        <v>1175995</v>
+      </c>
+      <c r="Q15" s="7">
+        <f t="shared" si="4"/>
+        <v>894110</v>
+      </c>
+      <c r="R15" s="5">
+        <v>0.78280000000000005</v>
+      </c>
+      <c r="S15" s="10">
+        <v>113440</v>
+      </c>
+      <c r="T15" s="10">
+        <f t="shared" si="5"/>
+        <v>47335</v>
+      </c>
+      <c r="U15" s="10">
+        <v>0.83830000000000005</v>
+      </c>
     </row>
-    <row r="15" spans="1:15" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+    <row r="16" spans="1:21" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="12">
-        <v>14798</v>
-      </c>
-      <c r="C15" s="12">
+      <c r="B16" s="7">
+        <v>41245</v>
+      </c>
+      <c r="C16" s="7">
         <f t="shared" si="0"/>
-        <v>6594</v>
-      </c>
-      <c r="D15" s="17">
-        <v>0.8085</v>
-      </c>
-      <c r="E15" s="12">
+        <v>28156</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.79700000000000004</v>
+      </c>
+      <c r="E16" s="7">
         <v>6134</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F16" s="7">
         <f t="shared" si="1"/>
         <v>1246</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G16" s="5">
         <v>0.81799999999999995</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H16" s="7">
         <v>402806</v>
       </c>
-      <c r="I15" s="12">
+      <c r="I16" s="7">
         <f t="shared" si="2"/>
         <v>340687</v>
       </c>
-      <c r="J15" s="7">
+      <c r="J16" s="5">
         <v>0.78500000000000003</v>
       </c>
-      <c r="K15" s="7">
+      <c r="K16" s="5">
         <v>0.7762</v>
       </c>
-      <c r="L15" s="12">
+      <c r="L16" s="7">
         <v>27</v>
       </c>
-      <c r="M15" s="12">
+      <c r="M16" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N15" s="7">
+      <c r="N16" s="5">
         <v>0.77239999999999998</v>
       </c>
-      <c r="O15" s="7">
+      <c r="O16" s="5">
         <v>0.74639999999999995</v>
       </c>
+      <c r="P16" s="7">
+        <v>3631310</v>
+      </c>
+      <c r="Q16" s="7">
+        <f t="shared" si="4"/>
+        <v>2455315</v>
+      </c>
+      <c r="R16" s="5">
+        <v>0.75890000000000002</v>
+      </c>
+      <c r="S16" s="10">
+        <v>373785</v>
+      </c>
+      <c r="T16" s="10">
+        <f t="shared" si="5"/>
+        <v>260345</v>
+      </c>
+      <c r="U16" s="10">
+        <v>0.81740000000000002</v>
+      </c>
     </row>
-    <row r="16" spans="1:15" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+    <row r="17" spans="1:21" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="12">
-        <v>37762</v>
-      </c>
-      <c r="C16" s="12">
+      <c r="B17" s="7">
+        <v>166845</v>
+      </c>
+      <c r="C17" s="7">
         <f t="shared" si="0"/>
-        <v>22964</v>
-      </c>
-      <c r="D16" s="7">
-        <v>0.80030000000000001</v>
-      </c>
-      <c r="E16" s="12">
+        <v>125600</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.80079999999999996</v>
+      </c>
+      <c r="E17" s="7">
         <v>8934</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F17" s="7">
         <f t="shared" si="1"/>
         <v>2800</v>
       </c>
-      <c r="G16" s="17">
+      <c r="G17" s="9">
         <v>0.8175</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H17" s="7">
         <v>1229422</v>
       </c>
-      <c r="I16" s="12">
+      <c r="I17" s="7">
         <f t="shared" si="2"/>
         <v>826616</v>
       </c>
-      <c r="J16" s="7">
+      <c r="J17" s="5">
         <v>0.78410000000000002</v>
       </c>
-      <c r="K16" s="7">
+      <c r="K17" s="5">
         <v>0.78010000000000002</v>
       </c>
-      <c r="L16" s="12">
+      <c r="L17" s="7">
         <v>27</v>
       </c>
-      <c r="M16" s="12">
+      <c r="M17" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N16" s="7">
+      <c r="N17" s="5">
         <v>0.77239999999999998</v>
       </c>
-      <c r="O16" s="7">
+      <c r="O17" s="5">
         <v>0.74639999999999995</v>
       </c>
+      <c r="P17" s="7">
+        <v>5857315</v>
+      </c>
+      <c r="Q17" s="7">
+        <f t="shared" si="4"/>
+        <v>2226005</v>
+      </c>
+      <c r="R17" s="5">
+        <v>0.75629999999999997</v>
+      </c>
+      <c r="S17" s="10">
+        <v>781925</v>
+      </c>
+      <c r="T17" s="10">
+        <f t="shared" si="5"/>
+        <v>408140</v>
+      </c>
+      <c r="U17" s="10">
+        <v>0.80430000000000001</v>
+      </c>
     </row>
-    <row r="17" spans="1:15" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+    <row r="18" spans="1:21" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="12">
-        <v>190196</v>
-      </c>
-      <c r="C17" s="12">
+      <c r="B18" s="7">
+        <v>891848</v>
+      </c>
+      <c r="C18" s="7">
         <f t="shared" si="0"/>
-        <v>152434</v>
-      </c>
-      <c r="D17" s="7">
-        <v>0.79800000000000004</v>
-      </c>
-      <c r="E17" s="12">
+        <v>725003</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0.78949999999999998</v>
+      </c>
+      <c r="E18" s="7">
         <v>19994</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F18" s="7">
         <f t="shared" si="1"/>
         <v>11060</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G18" s="5">
         <v>0.80830000000000002</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H18" s="7">
         <v>1539827</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I18" s="7">
         <f t="shared" si="2"/>
         <v>310405</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J18" s="5">
         <v>0.76839999999999997</v>
       </c>
-      <c r="K17" s="7">
+      <c r="K18" s="5">
         <v>0.76319999999999999</v>
       </c>
-      <c r="L17" s="12">
+      <c r="L18" s="7">
         <v>27</v>
       </c>
-      <c r="M17" s="12">
+      <c r="M18" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N17" s="7">
+      <c r="N18" s="5">
         <v>0.77239999999999998</v>
       </c>
-      <c r="O17" s="7">
+      <c r="O18" s="5">
         <v>0.74639999999999995</v>
       </c>
+      <c r="P18" s="7">
+        <v>7184630</v>
+      </c>
+      <c r="Q18" s="7">
+        <f t="shared" si="4"/>
+        <v>1327315</v>
+      </c>
+      <c r="R18" s="5">
+        <v>0.73050000000000004</v>
+      </c>
+      <c r="S18" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="T18" s="10" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U18" s="10">
+        <v>0.80740000000000001</v>
+      </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
     </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B29" s="2"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="H6:K6"/>
+  <mergeCells count="42">
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="S6:U6"/>
+    <mergeCell ref="S7:U7"/>
     <mergeCell ref="L1:O1"/>
     <mergeCell ref="L2:O2"/>
-    <mergeCell ref="L3:O3"/>
     <mergeCell ref="L4:O4"/>
     <mergeCell ref="L5:O5"/>
     <mergeCell ref="L6:O6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:K3"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E3:G3"/>
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="B4:D4"/>
     <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
     <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="P6:R6"/>
+    <mergeCell ref="P7:R7"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="P5:R5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>